<commit_message>
Add a piece initial transformation
D->D.ini.dl before L
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Manchu Language\Modern font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7768E9-162F-448F-B2BE-00EB6FBD1E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E03601-5927-4C44-BA99-1453356D87AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16824" yWindow="0" windowWidth="6312" windowHeight="12336" firstSheet="2" activeTab="2" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="16824" yWindow="0" windowWidth="6312" windowHeight="12336" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="139">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -566,6 +566,10 @@
   </si>
   <si>
     <t>V.fin.bv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D.init.dl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -973,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1271,61 +1275,61 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" t="s">
         <v>28</v>
-      </c>
-      <c r="B33" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,7 +1337,10 @@
         <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1341,10 +1348,7 @@
         <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
-      </c>
-      <c r="C41" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1352,21 +1356,21 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,7 +1378,10 @@
         <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1382,10 +1389,7 @@
         <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1393,10 +1397,10 @@
         <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,21 +1408,21 @@
         <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1426,7 +1430,10 @@
         <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1434,10 +1441,7 @@
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1445,10 +1449,10 @@
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1456,23 +1460,26 @@
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>109</v>
+      </c>
+      <c r="C53" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" t="s">
         <v>72</v>
@@ -1480,10 +1487,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1491,73 +1498,81 @@
         <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
-      </c>
-      <c r="C56" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>46</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1825,7 +1840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the doc and a corresponding correction of the font
finished isolated transformation. correct a glyph's name: I.coda->I.casemark
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Manchu Language\Modern font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEAE31D-51D3-4B80-ADD0-8DCB34D6B57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15CEE8E-98F3-4169-81EE-70B4DD8E6998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16824" yWindow="0" windowWidth="6312" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="285">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1125,6 +1125,10 @@
   </si>
   <si>
     <t>ZHs.med.ngzh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I.casemark</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2141,7 +2145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
@@ -3816,10 +3820,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0838EA3-FF44-4D74-A6B2-D370EFF4D086}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3846,220 +3850,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>46</v>
+        <v>284</v>
+      </c>
+      <c r="D2" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit the OT feature
Added the isolated transformation of case mark I
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Manchu Language\Modern font\GitHub\ManchuTextFont\Contribution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2F95C2-AD55-4AAC-81CA-1DEBC434EE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C146476-8C61-48EB-92C2-2B463DEFBBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15336" yWindow="0" windowWidth="7800" windowHeight="12336" firstSheet="5" activeTab="5" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="295">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1577,18 +1577,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>33</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>98</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>34</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>41</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>44</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>45</v>
       </c>
@@ -2191,15 +2191,15 @@
       <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>191</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>191</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>8</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>9</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>12</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>13</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>191</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>15</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>15</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>16</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>16</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>17</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>17</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>18</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>18</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>19</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>19</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>20</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>20</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>21</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>22</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>23</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>24</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>25</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>25</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>25</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>121</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>121</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>26</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>26</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>26</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>121</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>121</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>27</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>121</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>28</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>29</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>30</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>31</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>32</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>191</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>121</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>33</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>33</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>33</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>33</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>121</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>121</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>98</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>98</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>98</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>98</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>121</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>121</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>98</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>98</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>34</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>34</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>34</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>34</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>121</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>121</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>34</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>35</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>36</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>37</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>37</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>121</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>38</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>121</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>39</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>121</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>40</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>41</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>42</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>43</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>44</v>
       </c>
@@ -3238,7 +3238,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>45</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>121</v>
       </c>
@@ -3274,16 +3274,16 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>121</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -3360,7 +3360,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>121</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>121</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>121</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>13</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>14</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>14</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>15</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>16</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>17</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>18</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>19</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>20</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>22</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>23</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>23</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>24</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>24</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>25</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>26</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>27</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>28</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>29</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>30</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>31</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>32</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>33</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>98</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>98</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>34</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>35</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>36</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>37</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>38</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>39</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>40</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>41</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>42</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>42</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>43</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>44</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>45</v>
       </c>
@@ -3875,21 +3875,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0838EA3-FF44-4D74-A6B2-D370EFF4D086}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -3911,6 +3911,17 @@
         <v>283</v>
       </c>
       <c r="D2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3926,15 +3937,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3942,7 +3953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>235</v>
       </c>
@@ -3953,7 +3964,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>238</v>
       </c>
@@ -3964,7 +3975,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>235</v>
       </c>
@@ -3975,7 +3986,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -3989,7 +4000,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -4003,7 +4014,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -4017,7 +4028,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -4031,7 +4042,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -4045,7 +4056,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -4059,7 +4070,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -4073,7 +4084,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -4087,7 +4098,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -4101,7 +4112,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -4115,7 +4126,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -4129,7 +4140,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -4143,7 +4154,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -4157,7 +4168,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -4171,7 +4182,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -4185,7 +4196,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>109</v>
       </c>
@@ -4199,7 +4210,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>111</v>
       </c>
@@ -4213,7 +4224,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -4227,7 +4238,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -4241,7 +4252,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -4255,7 +4266,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -4269,7 +4280,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>77</v>
       </c>
@@ -4283,7 +4294,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -4297,7 +4308,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>290</v>
       </c>
@@ -4311,7 +4322,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>81</v>
       </c>
@@ -4325,7 +4336,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -4339,7 +4350,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -4353,7 +4364,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -4367,7 +4378,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -4381,7 +4392,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -4395,7 +4406,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -4409,7 +4420,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>57</v>
       </c>
@@ -4423,7 +4434,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -4437,7 +4448,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>59</v>
       </c>
@@ -4451,7 +4462,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>60</v>
       </c>
@@ -4465,7 +4476,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>68</v>
       </c>
@@ -4479,7 +4490,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -4493,7 +4504,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -4507,7 +4518,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -4521,7 +4532,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -4535,7 +4546,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>111</v>
       </c>
@@ -4549,7 +4560,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -4563,7 +4574,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -4577,7 +4588,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -4591,7 +4602,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -4605,7 +4616,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -4619,7 +4630,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -4633,7 +4644,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>290</v>
       </c>
@@ -4657,19 +4668,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5A95EF-6DA0-47A4-AC14-ECC198A340E1}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>293</v>
       </c>
@@ -4677,7 +4688,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -4685,7 +4696,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>193</v>
       </c>
@@ -4693,7 +4704,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>194</v>
       </c>
@@ -4701,7 +4712,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -4709,7 +4720,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -4717,7 +4728,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>196</v>
       </c>
@@ -4725,7 +4736,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>197</v>
       </c>
@@ -4733,7 +4744,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>198</v>
       </c>
@@ -4741,17 +4752,17 @@
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
Exchanged the romanization of IE and IY
For IE being better to represent the phoneme /ɯ/
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3140FD3A-BEFE-4DF9-81DC-15A40EEAFB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2AE3C7-1880-49E5-9FC8-9F054AEED141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="362">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -335,10 +335,6 @@
     <t>ZH.init</t>
   </si>
   <si>
-    <t>IE.init.iel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>N.init.ne</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1355,9 +1351,6 @@
     <t>1872</t>
   </si>
   <si>
-    <t>IY</t>
-  </si>
-  <si>
     <t>185F</t>
   </si>
   <si>
@@ -1368,6 +1361,18 @@
   </si>
   <si>
     <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IY.init.iyl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IY.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IY.med.miy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1789,21 +1794,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01EC8440-2A53-4A02-B21B-8604D35EC6F2}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B2" s="5">
         <v>1820</v>
@@ -1811,15 +1818,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>297</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B4" s="5">
         <v>1873</v>
@@ -1827,15 +1834,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B6" s="5">
         <v>1823</v>
@@ -1843,7 +1850,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B7" s="5">
         <v>1860</v>
@@ -1851,7 +1858,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B8" s="5">
         <v>1861</v>
@@ -1859,15 +1866,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B10" s="5">
         <v>1828</v>
@@ -1875,7 +1882,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B11" s="5">
         <v>1829</v>
@@ -1883,23 +1890,23 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B14" s="5">
         <v>1866</v>
@@ -1907,7 +1914,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B15" s="5">
         <v>1874</v>
@@ -1915,15 +1922,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>315</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B17" s="5">
         <v>1864</v>
@@ -1931,7 +1938,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B18" s="5">
         <v>1865</v>
@@ -1939,7 +1946,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B19" s="5">
         <v>1830</v>
@@ -1947,7 +1954,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B20" s="5">
         <v>1867</v>
@@ -1955,7 +1962,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B21" s="5">
         <v>1868</v>
@@ -1963,7 +1970,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B22" s="5">
         <v>1869</v>
@@ -1971,23 +1978,23 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>325</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B25" s="5">
         <v>1834</v>
@@ -1995,7 +2002,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B26" s="5">
         <v>1835</v>
@@ -2003,15 +2010,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>329</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B28" s="5">
         <v>1836</v>
@@ -2019,31 +2026,31 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>336</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B32" s="5">
         <v>1875</v>
@@ -2051,7 +2058,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B33" s="5">
         <v>1837</v>
@@ -2059,7 +2066,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B34" s="5">
         <v>1876</v>
@@ -2067,15 +2074,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B36" s="5">
         <v>1838</v>
@@ -2083,50 +2090,50 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>344</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>346</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>350</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>352</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>354</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2134,15 +2141,15 @@
         <v>356</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2163,9 +2170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2262,26 +2267,26 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>359</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
@@ -2300,7 +2305,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -2311,7 +2316,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
@@ -2330,7 +2335,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2338,7 +2343,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2346,10 +2351,10 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2357,7 +2362,7 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2365,10 +2370,10 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2384,7 +2389,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2432,10 +2437,10 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2451,10 +2456,10 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
         <v>90</v>
-      </c>
-      <c r="C32" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2462,7 +2467,7 @@
         <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
@@ -2521,10 +2526,10 @@
         <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2532,7 +2537,7 @@
         <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2540,10 +2545,10 @@
         <v>33</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2551,7 +2556,7 @@
         <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -2559,40 +2564,40 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
         <v>98</v>
       </c>
-      <c r="B44" t="s">
-        <v>99</v>
-      </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
@@ -2600,10 +2605,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C48" t="s">
         <v>27</v>
@@ -2614,10 +2619,10 @@
         <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2625,7 +2630,7 @@
         <v>34</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2633,10 +2638,10 @@
         <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2644,7 +2649,7 @@
         <v>34</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -2655,7 +2660,7 @@
         <v>34</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
         <v>27</v>
@@ -2690,10 +2695,10 @@
         <v>37</v>
       </c>
       <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" t="s">
         <v>109</v>
-      </c>
-      <c r="C57" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2701,7 +2706,7 @@
         <v>38</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2757,10 +2762,10 @@
         <v>45</v>
       </c>
       <c r="B65" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D65" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2771,10 +2776,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2804,7 +2809,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2812,29 +2817,29 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2845,7 +2850,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2856,7 +2861,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2864,29 +2869,29 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2894,29 +2899,29 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2924,18 +2929,18 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2943,40 +2948,40 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2987,7 +2992,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2998,7 +3003,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3006,7 +3011,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -3017,18 +3022,18 @@
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3036,37 +3041,34 @@
         <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>212</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>191</v>
-      </c>
       <c r="B29" t="s">
         <v>14</v>
       </c>
@@ -3075,11 +3077,14 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>190</v>
+      </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3087,18 +3092,18 @@
         <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>214</v>
-      </c>
-      <c r="D31" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
         <v>213</v>
+      </c>
+      <c r="D32" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -3106,18 +3111,18 @@
         <v>16</v>
       </c>
       <c r="C33" t="s">
-        <v>214</v>
-      </c>
-      <c r="D33" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>217</v>
+        <v>213</v>
+      </c>
+      <c r="D34" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -3127,16 +3132,16 @@
       <c r="C35" t="s">
         <v>216</v>
       </c>
-      <c r="D35" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>218</v>
+        <v>215</v>
+      </c>
+      <c r="D36" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -3144,21 +3149,18 @@
         <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>219</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D38" t="s">
-        <v>191</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -3166,18 +3168,18 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="D39" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
         <v>220</v>
-      </c>
-      <c r="D40" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -3185,47 +3187,50 @@
         <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>222</v>
+        <v>219</v>
+      </c>
+      <c r="D41" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -3233,10 +3238,7 @@
         <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>227</v>
-      </c>
-      <c r="D47" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -3244,52 +3246,55 @@
         <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D48" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>121</v>
-      </c>
       <c r="B49" t="s">
         <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>275</v>
+        <v>227</v>
       </c>
       <c r="D49" t="s">
         <v>230</v>
       </c>
-      <c r="E49" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
         <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E50" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>120</v>
+      </c>
       <c r="B51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C51" t="s">
-        <v>232</v>
+        <v>275</v>
+      </c>
+      <c r="D51" t="s">
+        <v>230</v>
+      </c>
+      <c r="E51" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -3297,10 +3302,7 @@
         <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>233</v>
-      </c>
-      <c r="D52" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -3308,161 +3310,164 @@
         <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D53" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>121</v>
-      </c>
       <c r="B54" t="s">
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>273</v>
+        <v>233</v>
       </c>
       <c r="D54" t="s">
         <v>230</v>
       </c>
-      <c r="E54" t="s">
-        <v>277</v>
-      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B55" t="s">
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D55" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E55" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>120</v>
+      </c>
       <c r="B56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C56" t="s">
-        <v>235</v>
+        <v>273</v>
+      </c>
+      <c r="D56" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>121</v>
-      </c>
       <c r="B57" t="s">
         <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>121</v>
-      </c>
       <c r="B59" t="s">
         <v>28</v>
       </c>
       <c r="C59" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
       <c r="B60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>121</v>
-      </c>
       <c r="B63" t="s">
         <v>31</v>
       </c>
       <c r="C63" t="s">
-        <v>280</v>
-      </c>
-      <c r="E63" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>120</v>
+      </c>
       <c r="B64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C64" t="s">
-        <v>243</v>
+        <v>279</v>
+      </c>
+      <c r="E64" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>191</v>
-      </c>
       <c r="B65" t="s">
         <v>32</v>
       </c>
       <c r="C65" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>190</v>
       </c>
       <c r="B66" t="s">
         <v>32</v>
       </c>
       <c r="C66" t="s">
-        <v>279</v>
-      </c>
-      <c r="E66" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>120</v>
+      </c>
       <c r="B67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C67" t="s">
-        <v>246</v>
+        <v>278</v>
+      </c>
+      <c r="E67" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -3472,19 +3477,16 @@
       <c r="C68" t="s">
         <v>245</v>
       </c>
-      <c r="D68" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>33</v>
       </c>
       <c r="C69" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
@@ -3492,358 +3494,369 @@
         <v>33</v>
       </c>
       <c r="C70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D70" t="s">
-        <v>249</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>121</v>
-      </c>
       <c r="B71" t="s">
         <v>33</v>
       </c>
       <c r="C71" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D71" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B72" t="s">
         <v>33</v>
       </c>
       <c r="C72" t="s">
+        <v>249</v>
+      </c>
+      <c r="D72" t="s">
         <v>251</v>
       </c>
-      <c r="D72" t="s">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" t="s">
+        <v>250</v>
+      </c>
+      <c r="D73" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>98</v>
-      </c>
-      <c r="C73" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C74" t="s">
-        <v>254</v>
-      </c>
-      <c r="D74" t="s">
-        <v>4</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C75" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C76" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D76" t="s">
-        <v>249</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>121</v>
-      </c>
       <c r="B77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C77" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D77" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D78" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>120</v>
+      </c>
+      <c r="B79" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" t="s">
+        <v>257</v>
+      </c>
+      <c r="D79" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
-        <v>98</v>
-      </c>
-      <c r="C79" t="s">
-        <v>237</v>
-      </c>
-      <c r="D79" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C80" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="D80" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C81" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="D81" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>34</v>
       </c>
       <c r="C82" t="s">
-        <v>261</v>
-      </c>
-      <c r="D82" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>34</v>
       </c>
       <c r="C83" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>34</v>
       </c>
       <c r="C84" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D84" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>121</v>
-      </c>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>34</v>
       </c>
       <c r="C85" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D85" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B86" t="s">
         <v>34</v>
       </c>
       <c r="C86" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D86" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>120</v>
+      </c>
       <c r="B87" t="s">
         <v>34</v>
       </c>
       <c r="C87" t="s">
+        <v>264</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C88" t="s">
+        <v>265</v>
+      </c>
+      <c r="D88" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" t="s">
         <v>266</v>
       </c>
-      <c r="D87" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
-        <v>35</v>
-      </c>
-      <c r="C88" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
         <v>36</v>
       </c>
-      <c r="C89" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>37</v>
-      </c>
       <c r="C90" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>37</v>
       </c>
       <c r="C91" t="s">
-        <v>269</v>
-      </c>
-      <c r="D91" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>121</v>
-      </c>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>37</v>
       </c>
       <c r="C92" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+      <c r="D92" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>120</v>
+      </c>
       <c r="B93" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C93" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>121</v>
-      </c>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>38</v>
       </c>
       <c r="C94" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>120</v>
+      </c>
       <c r="B95" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C95" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>121</v>
-      </c>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>39</v>
       </c>
       <c r="C96" t="s">
-        <v>281</v>
-      </c>
-      <c r="E96" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>120</v>
+      </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C97" t="s">
-        <v>272</v>
+        <v>280</v>
+      </c>
+      <c r="E97" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C98" t="s">
-        <v>205</v>
+        <v>271</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C99" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C100" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C101" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C102" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>121</v>
-      </c>
       <c r="B103" t="s">
         <v>45</v>
       </c>
       <c r="C103" t="s">
-        <v>282</v>
-      </c>
-      <c r="E103" t="s">
-        <v>277</v>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>120</v>
+      </c>
+      <c r="B104" t="s">
+        <v>45</v>
+      </c>
+      <c r="C104" t="s">
+        <v>281</v>
+      </c>
+      <c r="E104" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -3883,7 +3896,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3891,18 +3904,18 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3910,40 +3923,40 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3954,7 +3967,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3965,7 +3978,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3973,18 +3986,18 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3992,18 +4005,18 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -4011,21 +4024,21 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -4033,40 +4046,40 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -4077,7 +4090,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -4085,18 +4098,18 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4104,18 +4117,18 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -4123,7 +4136,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -4131,7 +4144,7 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4139,7 +4152,7 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -4147,10 +4160,10 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -4158,7 +4171,7 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -4166,7 +4179,7 @@
         <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -4174,7 +4187,7 @@
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -4182,7 +4195,7 @@
         <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -4190,7 +4203,7 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -4198,7 +4211,7 @@
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -4206,7 +4219,7 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -4214,7 +4227,7 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -4222,7 +4235,7 @@
         <v>23</v>
       </c>
       <c r="C37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
@@ -4230,10 +4243,10 @@
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -4241,7 +4254,7 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -4249,10 +4262,10 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -4260,7 +4273,7 @@
         <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -4268,7 +4281,7 @@
         <v>26</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -4276,7 +4289,7 @@
         <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -4284,7 +4297,7 @@
         <v>28</v>
       </c>
       <c r="C44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -4292,7 +4305,7 @@
         <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
@@ -4300,7 +4313,7 @@
         <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -4308,7 +4321,7 @@
         <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -4316,7 +4329,7 @@
         <v>32</v>
       </c>
       <c r="C48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -4324,26 +4337,26 @@
         <v>33</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -4351,7 +4364,7 @@
         <v>34</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -4359,7 +4372,7 @@
         <v>35</v>
       </c>
       <c r="C53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -4367,7 +4380,7 @@
         <v>36</v>
       </c>
       <c r="C54" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
@@ -4375,7 +4388,7 @@
         <v>37</v>
       </c>
       <c r="C55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
@@ -4383,7 +4396,7 @@
         <v>38</v>
       </c>
       <c r="C56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -4391,7 +4404,7 @@
         <v>39</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
@@ -4399,7 +4412,7 @@
         <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
@@ -4407,7 +4420,7 @@
         <v>41</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
@@ -4415,7 +4428,7 @@
         <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
@@ -4423,10 +4436,10 @@
         <v>42</v>
       </c>
       <c r="C61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
@@ -4434,7 +4447,7 @@
         <v>43</v>
       </c>
       <c r="C62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
@@ -4442,7 +4455,7 @@
         <v>44</v>
       </c>
       <c r="C63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
@@ -4450,7 +4463,7 @@
         <v>45</v>
       </c>
       <c r="C64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -4494,10 +4507,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4505,10 +4518,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -4541,35 +4554,35 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4577,13 +4590,13 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4591,13 +4604,13 @@
         <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4605,13 +4618,13 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4619,13 +4632,13 @@
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4633,13 +4646,13 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
         <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4647,13 +4660,13 @@
         <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s">
         <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4661,13 +4674,13 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
         <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4675,13 +4688,13 @@
         <v>57</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
         <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4689,13 +4702,13 @@
         <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" t="s">
         <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4703,13 +4716,13 @@
         <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
         <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4717,13 +4730,13 @@
         <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4731,13 +4744,13 @@
         <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" t="s">
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -4745,13 +4758,13 @@
         <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" t="s">
         <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4759,13 +4772,13 @@
         <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" t="s">
         <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -4773,41 +4786,41 @@
         <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
         <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4815,13 +4828,13 @@
         <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
         <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4829,13 +4842,13 @@
         <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" t="s">
         <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -4843,13 +4856,13 @@
         <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
         <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -4857,13 +4870,13 @@
         <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" t="s">
         <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -4871,13 +4884,13 @@
         <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
         <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4885,41 +4898,41 @@
         <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C27" t="s">
         <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>289</v>
+      </c>
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" t="s">
+        <v>289</v>
+      </c>
+      <c r="D28" t="s">
         <v>290</v>
-      </c>
-      <c r="B28" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" t="s">
-        <v>290</v>
-      </c>
-      <c r="D28" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -4927,13 +4940,13 @@
         <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
         <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -4941,13 +4954,13 @@
         <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" t="s">
         <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -4955,13 +4968,13 @@
         <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
         <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -4969,13 +4982,13 @@
         <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
         <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -4983,13 +4996,13 @@
         <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
         <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -4997,13 +5010,13 @@
         <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -5011,13 +5024,13 @@
         <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
       </c>
       <c r="D36" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -5025,13 +5038,13 @@
         <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C37" t="s">
         <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -5039,13 +5052,13 @@
         <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" t="s">
         <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -5053,13 +5066,13 @@
         <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" t="s">
         <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -5067,13 +5080,13 @@
         <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" t="s">
         <v>68</v>
       </c>
       <c r="D40" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -5081,13 +5094,13 @@
         <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C41" t="s">
         <v>69</v>
       </c>
       <c r="D41" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -5095,13 +5108,13 @@
         <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C42" t="s">
         <v>70</v>
       </c>
       <c r="D42" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -5109,41 +5122,41 @@
         <v>71</v>
       </c>
       <c r="B43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C43" t="s">
         <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -5151,13 +5164,13 @@
         <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" t="s">
         <v>73</v>
       </c>
       <c r="D46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -5165,13 +5178,13 @@
         <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" t="s">
         <v>74</v>
       </c>
       <c r="D47" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -5179,13 +5192,13 @@
         <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" t="s">
         <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -5193,13 +5206,13 @@
         <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
         <v>76</v>
       </c>
       <c r="D49" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -5207,13 +5220,13 @@
         <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C50" t="s">
         <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -5221,27 +5234,27 @@
         <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
         <v>78</v>
       </c>
       <c r="D51" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D52" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -5268,10 +5281,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5279,23 +5292,23 @@
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
         <v>194</v>
-      </c>
-      <c r="B4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -5303,44 +5316,44 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -5350,7 +5363,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applied the new stratege
Procrastinate the curations to Rlig or the ultimately refining phase (I forgot the name). Hence the initial, medial, and final transformations include only 2 passes: one for special forms such as Ta, Te, one for general forms such as C, J
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,23 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC667F0F-5EA6-475B-971E-FC78F7FF8337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BAE973-843C-4CD0-8371-20E4AADBF313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
     <sheet name="Initial" sheetId="1" r:id="rId2"/>
-    <sheet name="Spec-Init" sheetId="8" r:id="rId3"/>
-    <sheet name="Median" sheetId="2" r:id="rId4"/>
-    <sheet name="Final" sheetId="3" r:id="rId5"/>
-    <sheet name="Isolated" sheetId="4" r:id="rId6"/>
-    <sheet name="RLig" sheetId="5" r:id="rId7"/>
-    <sheet name="Kerning" sheetId="6" r:id="rId8"/>
+    <sheet name="Medial" sheetId="2" r:id="rId3"/>
+    <sheet name="Final" sheetId="3" r:id="rId4"/>
+    <sheet name="Isolated" sheetId="4" r:id="rId5"/>
+    <sheet name="RLig" sheetId="5" r:id="rId6"/>
+    <sheet name="Kerning" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Initial!$A$1:$D$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Spec-Init'!$A$1:$I$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Initial!$A$1:$C$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Medial!$A$1:$E$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="366">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1373,26 +1372,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SUB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>This page is for optimizing the grouping of special initial transformations</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>✓</t>
+    <t>D.init.ta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T.init.ta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Curation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New glyph for NG above round letters is needed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F.med.ngfi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1425,18 +1433,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1445,19 +1443,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1476,7 +1462,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1498,20 +1484,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1522,6 +1514,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2209,11 +2205,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B57"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2234,7 +2229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2242,7 +2237,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2250,7 +2245,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2258,7 +2253,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2266,7 +2261,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2274,7 +2269,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2284,2001 +2279,1219 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>357</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>100</v>
+      </c>
+      <c r="C41" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
-      </c>
-      <c r="C47" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="C50" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
-      </c>
-      <c r="C57" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>39</v>
-      </c>
-      <c r="B59" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>40</v>
-      </c>
-      <c r="B60" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>41</v>
-      </c>
-      <c r="B61" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>43</v>
-      </c>
-      <c r="B63" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>45</v>
-      </c>
-      <c r="B65" t="s">
         <v>287</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D65" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C58" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}"/>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B2:B58">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>COUNTIF($B:$B, B2)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AE2473-305A-4764-8885-AD7FD2AD9FCE}">
-  <dimension ref="A1:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>360</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>361</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E13" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="C18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>218</v>
+      </c>
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" t="s">
+        <v>226</v>
+      </c>
+      <c r="D40" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" t="s">
+        <v>232</v>
+      </c>
+      <c r="D43" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>233</v>
+      </c>
+      <c r="D44" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="C45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" t="s">
+        <v>246</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>247</v>
+      </c>
+      <c r="D54" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="C55" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" t="s">
+        <v>254</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>258</v>
+      </c>
+      <c r="D59" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="C60" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C61" t="s">
+        <v>260</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" t="s">
+        <v>261</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="s">
+        <v>262</v>
+      </c>
+      <c r="D63" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>37</v>
+      </c>
+      <c r="C67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>39</v>
+      </c>
+      <c r="C69" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>43</v>
+      </c>
+      <c r="C73" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>190</v>
+      </c>
+      <c r="B76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C76" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>190</v>
+      </c>
+      <c r="B77" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" t="s">
-        <v>363</v>
-      </c>
-      <c r="G12" t="s">
-        <v>363</v>
-      </c>
-      <c r="H12" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" t="s">
-        <v>363</v>
-      </c>
-      <c r="G13" t="s">
-        <v>363</v>
-      </c>
-      <c r="H13" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>93</v>
-      </c>
-      <c r="F16" t="s">
-        <v>363</v>
-      </c>
-      <c r="G16" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" t="s">
-        <v>363</v>
-      </c>
-      <c r="G18" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" t="s">
-        <v>363</v>
-      </c>
-      <c r="G20" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" t="s">
-        <v>363</v>
-      </c>
-      <c r="F22" t="s">
-        <v>363</v>
-      </c>
-      <c r="G22" t="s">
-        <v>363</v>
-      </c>
-      <c r="H22" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
-        <v>362</v>
+      <c r="C77" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I22" xr:uid="{49AE2473-305A-4764-8885-AD7FD2AD9FCE}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I22">
-      <sortCondition ref="I1:I22"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:E77" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
-  <dimension ref="A1:D104"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="11.75" customWidth="1"/>
-    <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>190</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>120</v>
-      </c>
-      <c r="B24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>190</v>
-      </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" t="s">
-        <v>213</v>
-      </c>
-      <c r="D32" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" t="s">
-        <v>213</v>
-      </c>
-      <c r="D34" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>17</v>
-      </c>
-      <c r="C36" t="s">
-        <v>215</v>
-      </c>
-      <c r="D36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" t="s">
-        <v>218</v>
-      </c>
-      <c r="D38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" t="s">
-        <v>219</v>
-      </c>
-      <c r="D39" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" t="s">
-        <v>219</v>
-      </c>
-      <c r="D41" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" t="s">
-        <v>226</v>
-      </c>
-      <c r="D48" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" t="s">
-        <v>227</v>
-      </c>
-      <c r="D49" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>120</v>
-      </c>
-      <c r="B50" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" t="s">
-        <v>274</v>
-      </c>
-      <c r="D50" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" t="s">
-        <v>275</v>
-      </c>
-      <c r="D51" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>26</v>
-      </c>
-      <c r="C52" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>26</v>
-      </c>
-      <c r="C53" t="s">
-        <v>232</v>
-      </c>
-      <c r="D53" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" t="s">
-        <v>233</v>
-      </c>
-      <c r="D54" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" t="s">
-        <v>272</v>
-      </c>
-      <c r="D55" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>120</v>
-      </c>
-      <c r="B56" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" t="s">
-        <v>273</v>
-      </c>
-      <c r="D56" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>27</v>
-      </c>
-      <c r="C57" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" t="s">
-        <v>27</v>
-      </c>
-      <c r="C58" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>28</v>
-      </c>
-      <c r="C59" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" t="s">
-        <v>28</v>
-      </c>
-      <c r="C60" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>29</v>
-      </c>
-      <c r="C61" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>31</v>
-      </c>
-      <c r="C63" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" t="s">
-        <v>31</v>
-      </c>
-      <c r="C64" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>190</v>
-      </c>
-      <c r="B66" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" t="s">
-        <v>32</v>
-      </c>
-      <c r="C67" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>33</v>
-      </c>
-      <c r="C68" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
-        <v>33</v>
-      </c>
-      <c r="C69" t="s">
-        <v>244</v>
-      </c>
-      <c r="D69" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
-        <v>33</v>
-      </c>
-      <c r="C70" t="s">
-        <v>246</v>
-      </c>
-      <c r="D70" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" t="s">
-        <v>247</v>
-      </c>
-      <c r="D71" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>120</v>
-      </c>
-      <c r="B72" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" t="s">
-        <v>249</v>
-      </c>
-      <c r="D72" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>120</v>
-      </c>
-      <c r="B73" t="s">
-        <v>33</v>
-      </c>
-      <c r="C73" t="s">
-        <v>250</v>
-      </c>
-      <c r="D73" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
-        <v>97</v>
-      </c>
-      <c r="C74" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" t="s">
-        <v>253</v>
-      </c>
-      <c r="D75" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
-        <v>97</v>
-      </c>
-      <c r="C76" t="s">
-        <v>254</v>
-      </c>
-      <c r="D76" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
-        <v>97</v>
-      </c>
-      <c r="C77" t="s">
-        <v>255</v>
-      </c>
-      <c r="D77" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>120</v>
-      </c>
-      <c r="B78" t="s">
-        <v>97</v>
-      </c>
-      <c r="C78" t="s">
-        <v>256</v>
-      </c>
-      <c r="D78" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>120</v>
-      </c>
-      <c r="B79" t="s">
-        <v>97</v>
-      </c>
-      <c r="C79" t="s">
-        <v>257</v>
-      </c>
-      <c r="D79" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
-        <v>97</v>
-      </c>
-      <c r="C80" t="s">
-        <v>236</v>
-      </c>
-      <c r="D80" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" t="s">
-        <v>258</v>
-      </c>
-      <c r="D81" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
-        <v>34</v>
-      </c>
-      <c r="C82" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
-        <v>34</v>
-      </c>
-      <c r="C83" t="s">
-        <v>260</v>
-      </c>
-      <c r="D83" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
-        <v>34</v>
-      </c>
-      <c r="C84" t="s">
-        <v>261</v>
-      </c>
-      <c r="D84" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
-        <v>34</v>
-      </c>
-      <c r="C85" t="s">
-        <v>262</v>
-      </c>
-      <c r="D85" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>120</v>
-      </c>
-      <c r="B86" t="s">
-        <v>34</v>
-      </c>
-      <c r="C86" t="s">
-        <v>263</v>
-      </c>
-      <c r="D86" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>120</v>
-      </c>
-      <c r="B87" t="s">
-        <v>34</v>
-      </c>
-      <c r="C87" t="s">
-        <v>264</v>
-      </c>
-      <c r="D87" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
-        <v>34</v>
-      </c>
-      <c r="C88" t="s">
-        <v>265</v>
-      </c>
-      <c r="D88" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
-        <v>35</v>
-      </c>
-      <c r="C89" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>36</v>
-      </c>
-      <c r="C90" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
-        <v>37</v>
-      </c>
-      <c r="C91" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
-        <v>37</v>
-      </c>
-      <c r="C92" t="s">
-        <v>268</v>
-      </c>
-      <c r="D92" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>120</v>
-      </c>
-      <c r="B93" t="s">
-        <v>37</v>
-      </c>
-      <c r="C93" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
-        <v>38</v>
-      </c>
-      <c r="C94" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>120</v>
-      </c>
-      <c r="B95" t="s">
-        <v>38</v>
-      </c>
-      <c r="C95" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
-        <v>39</v>
-      </c>
-      <c r="C96" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>120</v>
-      </c>
-      <c r="B97" t="s">
-        <v>39</v>
-      </c>
-      <c r="C97" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
-        <v>40</v>
-      </c>
-      <c r="C98" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B99" t="s">
-        <v>41</v>
-      </c>
-      <c r="C99" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B100" t="s">
-        <v>42</v>
-      </c>
-      <c r="C100" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
-        <v>43</v>
-      </c>
-      <c r="C101" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
-        <v>44</v>
-      </c>
-      <c r="C102" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B103" t="s">
-        <v>45</v>
-      </c>
-      <c r="C103" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>120</v>
-      </c>
-      <c r="B104" t="s">
-        <v>45</v>
-      </c>
-      <c r="C104" t="s">
-        <v>279</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4880,7 +4093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0838EA3-FF44-4D74-A6B2-D370EFF4D086}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -4938,11 +4151,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68:E95"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5665,13 +4880,542 @@
         <v>289</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
+        <v>357</v>
+      </c>
+      <c r="C58" t="s">
+        <v>27</v>
+      </c>
+      <c r="D58" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" t="s">
+        <v>136</v>
+      </c>
+      <c r="C61" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" t="s">
+        <v>27</v>
+      </c>
+      <c r="D62" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s">
+        <v>185</v>
+      </c>
+      <c r="E68" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>186</v>
+      </c>
+      <c r="E69" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>198</v>
+      </c>
+      <c r="E70" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>199</v>
+      </c>
+      <c r="E71" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>199</v>
+      </c>
+      <c r="D72" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" t="s">
+        <v>213</v>
+      </c>
+      <c r="D73" t="s">
+        <v>214</v>
+      </c>
+      <c r="E73" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" t="s">
+        <v>213</v>
+      </c>
+      <c r="D74" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" t="s">
+        <v>274</v>
+      </c>
+      <c r="D75" t="s">
+        <v>229</v>
+      </c>
+      <c r="E75" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" t="s">
+        <v>275</v>
+      </c>
+      <c r="D76" t="s">
+        <v>230</v>
+      </c>
+      <c r="E76" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77" t="s">
+        <v>272</v>
+      </c>
+      <c r="D77" t="s">
+        <v>229</v>
+      </c>
+      <c r="E77" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78" t="s">
+        <v>273</v>
+      </c>
+      <c r="D78" t="s">
+        <v>230</v>
+      </c>
+      <c r="E78" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" t="s">
+        <v>238</v>
+      </c>
+      <c r="E80" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>120</v>
+      </c>
+      <c r="B81" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" t="s">
+        <v>277</v>
+      </c>
+      <c r="E81" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>120</v>
+      </c>
+      <c r="B82" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" t="s">
+        <v>276</v>
+      </c>
+      <c r="E82" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>120</v>
+      </c>
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83" t="s">
+        <v>249</v>
+      </c>
+      <c r="D83" t="s">
+        <v>251</v>
+      </c>
+      <c r="E83" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>120</v>
+      </c>
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" t="s">
+        <v>97</v>
+      </c>
+      <c r="C85" t="s">
+        <v>256</v>
+      </c>
+      <c r="D85" t="s">
+        <v>251</v>
+      </c>
+      <c r="E85" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>120</v>
+      </c>
+      <c r="B86" t="s">
+        <v>97</v>
+      </c>
+      <c r="C86" t="s">
+        <v>257</v>
+      </c>
+      <c r="D86" t="s">
+        <v>4</v>
+      </c>
+      <c r="E86" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87" t="s">
+        <v>236</v>
+      </c>
+      <c r="D87" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>120</v>
+      </c>
+      <c r="B88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C88" t="s">
+        <v>263</v>
+      </c>
+      <c r="D88" t="s">
+        <v>251</v>
+      </c>
+      <c r="E88" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" t="s">
+        <v>264</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90" t="s">
+        <v>265</v>
+      </c>
+      <c r="D90" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>120</v>
+      </c>
+      <c r="B91" t="s">
+        <v>37</v>
+      </c>
+      <c r="C91" t="s">
+        <v>269</v>
+      </c>
+      <c r="E91" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" t="s">
+        <v>37</v>
+      </c>
+      <c r="C92" t="s">
+        <v>365</v>
+      </c>
+      <c r="D92" t="s">
+        <v>109</v>
+      </c>
+      <c r="E92" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" t="s">
+        <v>269</v>
+      </c>
+      <c r="E93" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>120</v>
+      </c>
+      <c r="B94" t="s">
+        <v>39</v>
+      </c>
+      <c r="C94" t="s">
+        <v>278</v>
+      </c>
+      <c r="E94" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>120</v>
+      </c>
+      <c r="B95" t="s">
+        <v>45</v>
+      </c>
+      <c r="C95" t="s">
+        <v>279</v>
+      </c>
+      <c r="E95" t="s">
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B57:B63">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>COUNTIF($B:$B, B57)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5A95EF-6DA0-47A4-AC14-ECC198A340E1}">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added medial I and Is under vowels
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BAE973-843C-4CD0-8371-20E4AADBF313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65A4F12-CF63-4DC9-B108-8F260E7DE50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
@@ -2743,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2989,20 +2989,23 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="D25" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
         <v>212</v>
@@ -3010,10 +3013,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3021,18 +3024,18 @@
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>215</v>
-      </c>
-      <c r="D28" t="s">
-        <v>86</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3040,21 +3043,18 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>218</v>
-      </c>
-      <c r="D30" t="s">
-        <v>86</v>
+        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D31" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3062,18 +3062,18 @@
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="D32" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>219</v>
-      </c>
-      <c r="D33" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -3081,47 +3081,50 @@
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="D34" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -3129,10 +3132,7 @@
         <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>226</v>
-      </c>
-      <c r="D40" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -3140,18 +3140,21 @@
         <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+      <c r="D42" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -3159,10 +3162,7 @@
         <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>232</v>
-      </c>
-      <c r="D43" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -3170,77 +3170,80 @@
         <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+      <c r="D45" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C51" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D52" t="s">
-        <v>4</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -3248,10 +3251,7 @@
         <v>33</v>
       </c>
       <c r="C53" t="s">
-        <v>246</v>
-      </c>
-      <c r="D53" t="s">
-        <v>7</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -3259,29 +3259,32 @@
         <v>33</v>
       </c>
       <c r="C54" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D54" t="s">
-        <v>248</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>252</v>
+        <v>246</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D56" t="s">
-        <v>4</v>
+        <v>248</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -3289,10 +3292,7 @@
         <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>254</v>
-      </c>
-      <c r="D57" t="s">
-        <v>7</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
@@ -3300,10 +3300,10 @@
         <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D58" t="s">
-        <v>248</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
@@ -3311,29 +3311,32 @@
         <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D59" t="s">
-        <v>145</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C60" t="s">
-        <v>259</v>
+        <v>255</v>
+      </c>
+      <c r="D60" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
@@ -3341,10 +3344,7 @@
         <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>261</v>
-      </c>
-      <c r="D62" t="s">
-        <v>7</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
@@ -3352,131 +3352,131 @@
         <v>34</v>
       </c>
       <c r="C63" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D63" t="s">
-        <v>248</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" t="s">
+        <v>261</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" t="s">
+        <v>262</v>
+      </c>
+      <c r="D65" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
         <v>35</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
         <v>36</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C67" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
         <v>37</v>
-      </c>
-      <c r="C66" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
-        <v>37</v>
-      </c>
-      <c r="C67" t="s">
-        <v>268</v>
-      </c>
-      <c r="D67" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>38</v>
       </c>
       <c r="C68" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" t="s">
+        <v>268</v>
+      </c>
+      <c r="D69" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
         <v>39</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C71" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
         <v>40</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C72" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" t="s">
         <v>41</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
         <v>42</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C74" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" t="s">
         <v>43</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
         <v>44</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C76" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
         <v>45</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C77" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>190</v>
-      </c>
-      <c r="B76" t="s">
-        <v>32</v>
-      </c>
-      <c r="C76" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>190</v>
-      </c>
-      <c r="B77" t="s">
-        <v>14</v>
-      </c>
-      <c r="C77" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -3490,7 +3490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added medial E U with dots under rounds
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65A4F12-CF63-4DC9-B108-8F260E7DE50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39280C81-6769-44E8-8CFB-2A5D770D0D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="5" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="366">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2741,10 +2741,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2772,7 +2773,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -2780,7 +2781,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -2790,27 +2791,27 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2820,27 +2821,27 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -2848,29 +2849,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -2892,7 +2871,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -2902,38 +2881,38 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -2943,16 +2922,16 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>184</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -2960,7 +2939,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>13</v>
       </c>
@@ -2968,7 +2947,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -2976,7 +2955,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>12</v>
       </c>
@@ -2984,7 +2963,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -2992,7 +2971,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>14</v>
       </c>
@@ -3003,7 +2982,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -3011,7 +2990,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -3019,7 +2998,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -3027,7 +3006,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>17</v>
       </c>
@@ -3038,7 +3017,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>18</v>
       </c>
@@ -3046,7 +3025,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>18</v>
       </c>
@@ -3057,7 +3036,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>19</v>
       </c>
@@ -3068,7 +3047,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>19</v>
       </c>
@@ -3076,7 +3055,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>20</v>
       </c>
@@ -3087,7 +3066,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>20</v>
       </c>
@@ -3095,7 +3074,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>21</v>
       </c>
@@ -3103,7 +3082,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>22</v>
       </c>
@@ -3111,7 +3090,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>23</v>
       </c>
@@ -3119,7 +3098,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>24</v>
       </c>
@@ -3127,7 +3106,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>25</v>
       </c>
@@ -3135,7 +3114,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>25</v>
       </c>
@@ -3146,7 +3125,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>25</v>
       </c>
@@ -3157,7 +3136,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>26</v>
       </c>
@@ -3165,7 +3144,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>26</v>
       </c>
@@ -3176,7 +3155,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>26</v>
       </c>
@@ -3187,7 +3166,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>27</v>
       </c>
@@ -3195,7 +3174,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>28</v>
       </c>
@@ -3203,7 +3182,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>29</v>
       </c>
@@ -3211,7 +3190,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>30</v>
       </c>
@@ -3219,7 +3198,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>31</v>
       </c>
@@ -3227,7 +3206,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>32</v>
       </c>
@@ -3235,7 +3214,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>32</v>
       </c>
@@ -3246,7 +3225,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>33</v>
       </c>
@@ -3254,7 +3233,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>33</v>
       </c>
@@ -3265,7 +3244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>33</v>
       </c>
@@ -3276,7 +3255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>33</v>
       </c>
@@ -3287,7 +3266,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>97</v>
       </c>
@@ -3295,7 +3274,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>97</v>
       </c>
@@ -3306,7 +3285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>97</v>
       </c>
@@ -3317,7 +3296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>97</v>
       </c>
@@ -3328,7 +3307,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>97</v>
       </c>
@@ -3339,7 +3318,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>34</v>
       </c>
@@ -3347,7 +3326,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>34</v>
       </c>
@@ -3358,7 +3337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>34</v>
       </c>
@@ -3369,7 +3348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>34</v>
       </c>
@@ -3380,7 +3359,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>35</v>
       </c>
@@ -3388,7 +3367,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>36</v>
       </c>
@@ -3396,7 +3375,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>37</v>
       </c>
@@ -3404,7 +3383,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>37</v>
       </c>
@@ -3415,7 +3394,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>38</v>
       </c>
@@ -3423,7 +3402,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>39</v>
       </c>
@@ -3431,7 +3410,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>40</v>
       </c>
@@ -3439,7 +3418,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>41</v>
       </c>
@@ -3447,7 +3426,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>42</v>
       </c>
@@ -3455,7 +3434,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>43</v>
       </c>
@@ -3463,7 +3442,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>44</v>
       </c>
@@ -3471,7 +3450,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>45</v>
       </c>
@@ -3480,7 +3459,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E77" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}"/>
+  <autoFilter ref="A1:E77" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E19">
+      <sortCondition ref="A1:A77"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4153,10 +4141,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:E95"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5401,6 +5389,34 @@
         <v>279</v>
       </c>
       <c r="E95" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>120</v>
+      </c>
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" t="s">
+        <v>188</v>
+      </c>
+      <c r="E96" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>120</v>
+      </c>
+      <c r="B97" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" t="s">
+        <v>188</v>
+      </c>
+      <c r="E97" t="s">
         <v>362</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the final I
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39280C81-6769-44E8-8CFB-2A5D770D0D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF20F303-DCF4-4A6C-B87C-6257C6854CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="5" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
     <sheet name="Initial" sheetId="1" r:id="rId2"/>
     <sheet name="Medial" sheetId="2" r:id="rId3"/>
-    <sheet name="Final" sheetId="3" r:id="rId4"/>
-    <sheet name="Isolated" sheetId="4" r:id="rId5"/>
-    <sheet name="RLig" sheetId="5" r:id="rId6"/>
-    <sheet name="Kerning" sheetId="6" r:id="rId7"/>
+    <sheet name="Canvas" sheetId="10" r:id="rId4"/>
+    <sheet name="Final" sheetId="3" r:id="rId5"/>
+    <sheet name="Isolated" sheetId="4" r:id="rId6"/>
+    <sheet name="RLig" sheetId="5" r:id="rId7"/>
+    <sheet name="Kerning" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Initial!$A$1:$C$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Medial!$A$1:$E$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Medial!$A$1:$E$75</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="366">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1488,7 +1489,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2208,7 +2223,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2731,7 +2746,7 @@
   <autoFilter ref="A1:C58" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B58">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>COUNTIF($B:$B, B2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2742,10 +2757,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E11"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2753,7 +2768,7 @@
     <col min="1" max="1" width="19.25" customWidth="1"/>
     <col min="2" max="2" width="11.75" customWidth="1"/>
     <col min="3" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2773,7 +2788,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -2781,7 +2796,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -2789,7 +2804,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2800,7 +2815,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -2811,7 +2826,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -2819,7 +2834,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -2830,7 +2845,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -2841,199 +2856,218 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E11" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
-      </c>
-      <c r="E13" t="s">
-        <v>364</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
       <c r="C16" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>184</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>184</v>
-      </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+      <c r="D23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>211</v>
-      </c>
-      <c r="D25" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>215</v>
+        <v>260</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+      <c r="D30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>218</v>
-      </c>
-      <c r="D31" t="s">
-        <v>86</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
@@ -3047,82 +3081,82 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>219</v>
-      </c>
-      <c r="D34" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>225</v>
+        <v>219</v>
+      </c>
+      <c r="D39" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+      <c r="D40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>226</v>
-      </c>
-      <c r="D41" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
@@ -3130,10 +3164,10 @@
         <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
@@ -3141,118 +3175,118 @@
         <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+      <c r="D43" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>232</v>
-      </c>
-      <c r="D44" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+      <c r="D50" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D52" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>245</v>
+        <v>258</v>
+      </c>
+      <c r="D53" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="D54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="C55" t="s">
-        <v>246</v>
-      </c>
-      <c r="D55" t="s">
-        <v>7</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
@@ -3260,10 +3294,10 @@
         <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D56" t="s">
-        <v>248</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
@@ -3271,210 +3305,483 @@
         <v>97</v>
       </c>
       <c r="C57" t="s">
-        <v>252</v>
+        <v>254</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="D58" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="C59" t="s">
-        <v>254</v>
+        <v>215</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>255</v>
-      </c>
-      <c r="D60" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>97</v>
+        <v>18</v>
       </c>
       <c r="C61" t="s">
-        <v>258</v>
+        <v>218</v>
       </c>
       <c r="D61" t="s">
-        <v>145</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C62" t="s">
-        <v>259</v>
+        <v>247</v>
+      </c>
+      <c r="D62" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="63" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="C63" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D63" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C64" t="s">
-        <v>261</v>
-      </c>
-      <c r="D64" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
-        <v>34</v>
-      </c>
-      <c r="C65" t="s">
-        <v>262</v>
-      </c>
-      <c r="D65" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C67" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
-        <v>37</v>
-      </c>
-      <c r="C68" t="s">
+        <v>262</v>
+      </c>
+      <c r="D67" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C68" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="69" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C69" t="s">
-        <v>268</v>
-      </c>
-      <c r="D69" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C70" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C71" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C72" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C74" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C75" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
-        <v>44</v>
-      </c>
-      <c r="C76" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
-        <v>45</v>
-      </c>
-      <c r="C77" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E77" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
+  <autoFilter ref="A1:E75" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
     <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters blank="1"/>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:E19">
-      <sortCondition ref="A1:A77"/>
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:E67">
+      <sortCondition ref="D1:D75"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>COUNTIF($C:$C,C1)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C0AE4-7BC5-4B30-B89D-2A08841991C9}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>218</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
   <dimension ref="A1:E64"/>
   <sheetViews>
@@ -4081,7 +4388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0838EA3-FF44-4D74-A6B2-D370EFF4D086}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -4139,11 +4446,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
@@ -5423,7 +5730,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B57:B63">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>COUNTIF($B:$B, B57)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5431,7 +5738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5A95EF-6DA0-47A4-AC14-ECC198A340E1}">
   <dimension ref="A1:B12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added final O V under round letters
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF20F303-DCF4-4A6C-B87C-6257C6854CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A14AA6-000B-48EC-AC7A-8E3B11B42663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Kerning" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Final!$A$1:$E$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Initial!$A$1:$C$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Medial!$A$1:$E$75</definedName>
   </definedNames>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="366">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1463,7 +1464,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1483,6 +1484,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2746,7 +2750,7 @@
   <autoFilter ref="A1:C58" xr:uid="{0EE99D31-30A4-40C8-A7F0-F012C73A7348}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B58">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>COUNTIF($B:$B, B2)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2756,11 +2760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:XFD75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2804,7 +2807,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2815,7 +2818,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>190</v>
       </c>
@@ -2834,7 +2837,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -2905,7 +2908,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -2916,7 +2919,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>184</v>
       </c>
@@ -2986,7 +2989,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>33</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>97</v>
       </c>
@@ -3040,7 +3043,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>34</v>
       </c>
@@ -3051,7 +3054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>14</v>
       </c>
@@ -3070,7 +3073,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>19</v>
       </c>
@@ -3129,7 +3132,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>20</v>
       </c>
@@ -3140,7 +3143,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>32</v>
       </c>
@@ -3159,7 +3162,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>25</v>
       </c>
@@ -3170,7 +3173,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>26</v>
       </c>
@@ -3229,7 +3232,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>25</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>26</v>
       </c>
@@ -3259,7 +3262,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>97</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>37</v>
       </c>
@@ -3289,7 +3292,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>33</v>
       </c>
@@ -3300,7 +3303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>97</v>
       </c>
@@ -3311,7 +3314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>34</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>17</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="61" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>18</v>
       </c>
@@ -3352,7 +3355,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>33</v>
       </c>
@@ -3363,7 +3366,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="63" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>97</v>
       </c>
@@ -3398,7 +3401,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>34</v>
       </c>
@@ -3475,12 +3478,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E75" xr:uid="{FA182170-6922-4B0E-B039-5A332D90316A}">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters blank="1"/>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:E67">
       <sortCondition ref="D1:D75"/>
     </sortState>
@@ -3497,282 +3494,148 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C0AE4-7BC5-4B30-B89D-2A08841991C9}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>227</v>
-      </c>
-      <c r="D7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D8" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>268</v>
-      </c>
-      <c r="D9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="B11" s="6" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" t="s">
-        <v>258</v>
-      </c>
-      <c r="D19" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>215</v>
-      </c>
-      <c r="D20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>218</v>
-      </c>
-      <c r="D21" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3783,11 +3646,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3876,30 +3737,27 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
+      <c r="B8" t="s">
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
         <v>123</v>
@@ -3910,7 +3768,7 @@
         <v>120</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>124</v>
@@ -3918,10 +3776,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3929,460 +3787,431 @@
         <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>126</v>
+      </c>
+      <c r="E13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>122</v>
-      </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>286</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>120</v>
+      </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>120</v>
-      </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>120</v>
-      </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
+        <v>142</v>
+      </c>
+      <c r="D25" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>142</v>
-      </c>
-      <c r="D28" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>152</v>
+        <v>155</v>
+      </c>
+      <c r="D35" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>154</v>
+        <v>164</v>
+      </c>
+      <c r="D37" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
-      </c>
-      <c r="D38" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>177</v>
+      </c>
+      <c r="D48" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
-      </c>
-      <c r="D51" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C52" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C54" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>171</v>
+        <v>179</v>
+      </c>
+      <c r="D58" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C59" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C60" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>179</v>
-      </c>
-      <c r="D61" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" t="s">
         <v>176</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E61" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4448,10 +4277,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102:XFD102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5727,10 +5556,43 @@
         <v>362</v>
       </c>
     </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>28</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>14</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>14</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B57:B63">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>COUNTIF($B:$B, B57)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added the a-uju-alphabet form of final O U
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A14AA6-000B-48EC-AC7A-8E3B11B42663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77521C03-936E-42DE-AABE-B2E6431A6169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="6" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="362">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -265,12 +265,6 @@
     <t>SH.init</t>
   </si>
   <si>
-    <t>T.init</t>
-  </si>
-  <si>
-    <t>D.init</t>
-  </si>
-  <si>
     <t>L.init</t>
   </si>
   <si>
@@ -1147,14 +1141,6 @@
   </si>
   <si>
     <t>ZHs.init</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O.fin.Co</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>U.fin.Co</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1866,15 +1852,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B2" s="4">
         <v>1820</v>
@@ -1882,15 +1868,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B4" s="4">
         <v>1873</v>
@@ -1898,15 +1884,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B6" s="4">
         <v>1823</v>
@@ -1914,7 +1900,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B7" s="4">
         <v>1860</v>
@@ -1922,7 +1908,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B8" s="4">
         <v>1861</v>
@@ -1930,15 +1916,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B10" s="4">
         <v>1828</v>
@@ -1946,7 +1932,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B11" s="4">
         <v>1829</v>
@@ -1954,23 +1940,23 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B14" s="4">
         <v>1866</v>
@@ -1978,7 +1964,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B15" s="4">
         <v>1874</v>
@@ -1986,15 +1972,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B17" s="4">
         <v>1864</v>
@@ -2002,7 +1988,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B18" s="4">
         <v>1865</v>
@@ -2010,7 +1996,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B19" s="4">
         <v>1830</v>
@@ -2018,7 +2004,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B20" s="4">
         <v>1867</v>
@@ -2026,7 +2012,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B21" s="4">
         <v>1868</v>
@@ -2034,7 +2020,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B22" s="4">
         <v>1869</v>
@@ -2042,23 +2028,23 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B25" s="4">
         <v>1834</v>
@@ -2066,7 +2052,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B26" s="4">
         <v>1835</v>
@@ -2074,15 +2060,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B28" s="4">
         <v>1836</v>
@@ -2090,31 +2076,31 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B32" s="4">
         <v>1875</v>
@@ -2122,7 +2108,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B33" s="4">
         <v>1837</v>
@@ -2130,7 +2116,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B34" s="4">
         <v>1876</v>
@@ -2138,15 +2124,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B36" s="4">
         <v>1838</v>
@@ -2154,66 +2140,66 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2253,7 +2239,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2261,7 +2247,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2269,7 +2255,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2277,7 +2263,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2285,7 +2271,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2301,7 +2287,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2309,7 +2295,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2349,7 +2335,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2357,7 +2343,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2365,10 +2351,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2376,7 +2362,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2384,10 +2370,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2403,7 +2389,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2443,7 +2429,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2451,10 +2437,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
         <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2462,7 +2448,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2470,10 +2456,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2481,7 +2467,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2489,7 +2475,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2497,7 +2483,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2505,7 +2491,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2513,7 +2499,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2521,7 +2507,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2529,10 +2515,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2540,7 +2526,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2548,10 +2534,10 @@
         <v>33</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2559,7 +2545,7 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
@@ -2567,40 +2553,40 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
         <v>97</v>
-      </c>
-      <c r="B40" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
@@ -2611,10 +2597,10 @@
         <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2622,7 +2608,7 @@
         <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2630,10 +2616,10 @@
         <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2641,7 +2627,7 @@
         <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
@@ -2652,7 +2638,7 @@
         <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2660,7 +2646,7 @@
         <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2668,7 +2654,7 @@
         <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
@@ -2676,10 +2662,10 @@
         <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2687,7 +2673,7 @@
         <v>38</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2695,7 +2681,7 @@
         <v>39</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2703,7 +2689,7 @@
         <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2711,7 +2697,7 @@
         <v>41</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2719,7 +2705,7 @@
         <v>42</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2727,7 +2713,7 @@
         <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2735,7 +2721,7 @@
         <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2743,7 +2729,7 @@
         <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2788,7 +2774,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2796,7 +2782,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2804,29 +2790,29 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2834,29 +2820,29 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2864,7 +2850,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2872,21 +2858,21 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2894,40 +2880,40 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2935,18 +2921,18 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2954,7 +2940,7 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2962,7 +2948,7 @@
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2970,7 +2956,7 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2978,7 +2964,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2986,7 +2972,7 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2994,7 +2980,7 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -3005,7 +2991,7 @@
         <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3013,7 +2999,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3021,15 +3007,15 @@
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -3040,7 +3026,7 @@
         <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -3048,7 +3034,7 @@
         <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -3059,10 +3045,10 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3070,7 +3056,7 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3078,10 +3064,10 @@
         <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3089,7 +3075,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -3097,7 +3083,7 @@
         <v>21</v>
       </c>
       <c r="C34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -3105,7 +3091,7 @@
         <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -3113,7 +3099,7 @@
         <v>23</v>
       </c>
       <c r="C36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -3121,7 +3107,7 @@
         <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
@@ -3129,7 +3115,7 @@
         <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -3137,10 +3123,10 @@
         <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -3148,10 +3134,10 @@
         <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -3159,7 +3145,7 @@
         <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -3167,10 +3153,10 @@
         <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D42" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -3178,10 +3164,10 @@
         <v>26</v>
       </c>
       <c r="C43" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D43" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -3189,7 +3175,7 @@
         <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -3197,7 +3183,7 @@
         <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
@@ -3205,7 +3191,7 @@
         <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -3213,7 +3199,7 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3221,7 +3207,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -3229,7 +3215,7 @@
         <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -3237,10 +3223,10 @@
         <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D50" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
@@ -3248,7 +3234,7 @@
         <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -3256,21 +3242,21 @@
         <v>26</v>
       </c>
       <c r="C52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D52" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C53" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -3278,18 +3264,18 @@
         <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
@@ -3297,7 +3283,7 @@
         <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -3305,10 +3291,10 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C57" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -3319,7 +3305,7 @@
         <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -3330,10 +3316,10 @@
         <v>17</v>
       </c>
       <c r="C59" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D59" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
@@ -3341,7 +3327,7 @@
         <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
@@ -3349,10 +3335,10 @@
         <v>18</v>
       </c>
       <c r="C61" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D61" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
@@ -3360,21 +3346,21 @@
         <v>33</v>
       </c>
       <c r="C62" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D62" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D63" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
@@ -3382,7 +3368,7 @@
         <v>35</v>
       </c>
       <c r="C64" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3390,7 +3376,7 @@
         <v>36</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
@@ -3398,7 +3384,7 @@
         <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
@@ -3406,10 +3392,10 @@
         <v>34</v>
       </c>
       <c r="C67" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D67" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3417,7 +3403,7 @@
         <v>38</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
@@ -3425,7 +3411,7 @@
         <v>39</v>
       </c>
       <c r="C69" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
@@ -3433,7 +3419,7 @@
         <v>40</v>
       </c>
       <c r="C70" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
@@ -3441,7 +3427,7 @@
         <v>41</v>
       </c>
       <c r="C71" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
@@ -3449,7 +3435,7 @@
         <v>42</v>
       </c>
       <c r="C72" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
@@ -3457,7 +3443,7 @@
         <v>43</v>
       </c>
       <c r="C73" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
@@ -3465,7 +3451,7 @@
         <v>44</v>
       </c>
       <c r="C74" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
@@ -3473,7 +3459,7 @@
         <v>45</v>
       </c>
       <c r="C75" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3496,8 +3482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C0AE4-7BC5-4B30-B89D-2A08841991C9}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3508,134 +3494,134 @@
   <sheetData>
     <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3673,7 +3659,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3681,18 +3667,18 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3700,40 +3686,40 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -3741,18 +3727,18 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3760,18 +3746,18 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3779,21 +3765,21 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" t="s">
         <v>126</v>
-      </c>
-      <c r="E13" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3801,40 +3787,40 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3842,18 +3828,18 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3861,18 +3847,18 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3880,7 +3866,7 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3888,7 +3874,7 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -3896,7 +3882,7 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3904,10 +3890,10 @@
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3915,7 +3901,7 @@
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3923,7 +3909,7 @@
         <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3931,7 +3917,7 @@
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -3939,7 +3925,7 @@
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3947,7 +3933,7 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3955,7 +3941,7 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3963,7 +3949,7 @@
         <v>21</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
@@ -3971,7 +3957,7 @@
         <v>22</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -3979,7 +3965,7 @@
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -3987,10 +3973,10 @@
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D35" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
@@ -3998,7 +3984,7 @@
         <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -4006,10 +3992,10 @@
         <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
@@ -4017,7 +4003,7 @@
         <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -4025,7 +4011,7 @@
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
@@ -4033,7 +4019,7 @@
         <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -4041,7 +4027,7 @@
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
@@ -4049,7 +4035,7 @@
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
@@ -4057,7 +4043,7 @@
         <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -4065,7 +4051,7 @@
         <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -4073,7 +4059,7 @@
         <v>32</v>
       </c>
       <c r="C45" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
@@ -4081,26 +4067,26 @@
         <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -4108,7 +4094,7 @@
         <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -4116,7 +4102,7 @@
         <v>35</v>
       </c>
       <c r="C50" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
@@ -4124,7 +4110,7 @@
         <v>36</v>
       </c>
       <c r="C51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -4132,7 +4118,7 @@
         <v>37</v>
       </c>
       <c r="C52" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -4140,7 +4126,7 @@
         <v>38</v>
       </c>
       <c r="C53" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -4148,7 +4134,7 @@
         <v>39</v>
       </c>
       <c r="C54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
@@ -4156,7 +4142,7 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
@@ -4164,7 +4150,7 @@
         <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -4172,7 +4158,7 @@
         <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
@@ -4180,10 +4166,10 @@
         <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
@@ -4191,7 +4177,7 @@
         <v>43</v>
       </c>
       <c r="C59" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
@@ -4199,7 +4185,7 @@
         <v>44</v>
       </c>
       <c r="C60" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
@@ -4207,7 +4193,7 @@
         <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -4252,10 +4238,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4263,10 +4249,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -4277,10 +4263,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:XFD102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4301,1299 +4287,641 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>283</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>125</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>353</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>288</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>108</v>
-      </c>
-      <c r="B20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+      <c r="E21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="E22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+      <c r="E23" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="E24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>197</v>
       </c>
       <c r="D25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>77</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E25" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>125</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>211</v>
       </c>
       <c r="D26" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>78</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="E26" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>211</v>
       </c>
       <c r="D27" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="E27" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>287</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D28" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+      <c r="E28" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>285</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>273</v>
       </c>
       <c r="D29" t="s">
+        <v>228</v>
+      </c>
+      <c r="E29" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" t="s">
+        <v>227</v>
+      </c>
+      <c r="E30" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>271</v>
+      </c>
+      <c r="D31" t="s">
+        <v>228</v>
+      </c>
+      <c r="E31" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
+        <v>236</v>
+      </c>
+      <c r="E33" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>275</v>
+      </c>
+      <c r="E34" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>274</v>
+      </c>
+      <c r="E35" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>118</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>247</v>
+      </c>
+      <c r="D36" t="s">
+        <v>249</v>
+      </c>
+      <c r="E36" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>248</v>
+      </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" t="s">
+        <v>254</v>
+      </c>
+      <c r="D38" t="s">
+        <v>249</v>
+      </c>
+      <c r="E38" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" t="s">
+        <v>255</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>261</v>
+      </c>
+      <c r="D41" t="s">
+        <v>249</v>
+      </c>
+      <c r="E41" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>262</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>263</v>
+      </c>
+      <c r="D43" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>267</v>
+      </c>
+      <c r="E44" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>361</v>
+      </c>
+      <c r="D45" t="s">
+        <v>107</v>
+      </c>
+      <c r="E45" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>267</v>
+      </c>
+      <c r="E46" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>276</v>
+      </c>
+      <c r="E47" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" t="s">
+        <v>277</v>
+      </c>
+      <c r="E48" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>186</v>
+      </c>
+      <c r="E49" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>186</v>
+      </c>
+      <c r="E50" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
         <v>284</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" t="s">
-        <v>129</v>
-      </c>
-      <c r="C33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" t="s">
-        <v>129</v>
-      </c>
-      <c r="C35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" t="s">
-        <v>129</v>
-      </c>
-      <c r="C36" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
-        <v>129</v>
-      </c>
-      <c r="C39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>129</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C42" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>108</v>
-      </c>
-      <c r="B44" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" t="s">
-        <v>129</v>
-      </c>
-      <c r="C46" t="s">
-        <v>73</v>
-      </c>
-      <c r="D46" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D47" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" t="s">
-        <v>129</v>
-      </c>
-      <c r="C48" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>129</v>
-      </c>
-      <c r="C50" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" t="s">
-        <v>129</v>
-      </c>
-      <c r="C51" t="s">
-        <v>78</v>
-      </c>
-      <c r="D51" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>287</v>
-      </c>
-      <c r="B52" t="s">
-        <v>129</v>
-      </c>
-      <c r="C52" t="s">
-        <v>287</v>
-      </c>
-      <c r="D52" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>12</v>
-      </c>
-      <c r="B58" t="s">
-        <v>357</v>
-      </c>
-      <c r="C58" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>14</v>
-      </c>
-      <c r="B60" t="s">
-        <v>80</v>
-      </c>
-      <c r="C60" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" t="s">
-        <v>136</v>
-      </c>
-      <c r="C61" t="s">
-        <v>27</v>
-      </c>
-      <c r="D61" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" t="s">
-        <v>102</v>
-      </c>
-      <c r="C62" t="s">
-        <v>27</v>
-      </c>
-      <c r="D62" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>34</v>
-      </c>
-      <c r="B63" t="s">
-        <v>107</v>
-      </c>
-      <c r="C63" t="s">
-        <v>27</v>
-      </c>
-      <c r="D63" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>14</v>
-      </c>
-      <c r="B68" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" t="s">
-        <v>185</v>
-      </c>
-      <c r="E68" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" t="s">
-        <v>186</v>
-      </c>
-      <c r="E69" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>14</v>
-      </c>
-      <c r="B70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" t="s">
-        <v>198</v>
-      </c>
-      <c r="E70" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>28</v>
-      </c>
-      <c r="B71" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" t="s">
-        <v>199</v>
-      </c>
-      <c r="E71" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" t="s">
-        <v>199</v>
-      </c>
-      <c r="D72" t="s">
-        <v>27</v>
-      </c>
-      <c r="E72" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
-        <v>15</v>
-      </c>
-      <c r="C73" t="s">
-        <v>213</v>
-      </c>
-      <c r="D73" t="s">
-        <v>214</v>
-      </c>
-      <c r="E73" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
-        <v>16</v>
-      </c>
-      <c r="C74" t="s">
-        <v>213</v>
-      </c>
-      <c r="D74" t="s">
-        <v>214</v>
-      </c>
-      <c r="E74" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>120</v>
-      </c>
-      <c r="B75" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" t="s">
-        <v>274</v>
-      </c>
-      <c r="D75" t="s">
-        <v>229</v>
-      </c>
-      <c r="E75" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>120</v>
-      </c>
-      <c r="B76" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" t="s">
-        <v>275</v>
-      </c>
-      <c r="D76" t="s">
-        <v>230</v>
-      </c>
-      <c r="E76" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>120</v>
-      </c>
-      <c r="B77" t="s">
-        <v>26</v>
-      </c>
-      <c r="C77" t="s">
-        <v>272</v>
-      </c>
-      <c r="D77" t="s">
-        <v>229</v>
-      </c>
-      <c r="E77" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>120</v>
-      </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78" t="s">
-        <v>273</v>
-      </c>
-      <c r="D78" t="s">
-        <v>230</v>
-      </c>
-      <c r="E78" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>120</v>
-      </c>
-      <c r="B80" t="s">
-        <v>28</v>
-      </c>
-      <c r="C80" t="s">
-        <v>238</v>
-      </c>
-      <c r="E80" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>120</v>
-      </c>
-      <c r="B81" t="s">
-        <v>31</v>
-      </c>
-      <c r="C81" t="s">
-        <v>277</v>
-      </c>
-      <c r="E81" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>120</v>
-      </c>
-      <c r="B82" t="s">
-        <v>32</v>
-      </c>
-      <c r="C82" t="s">
-        <v>276</v>
-      </c>
-      <c r="E82" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>120</v>
-      </c>
-      <c r="B83" t="s">
-        <v>33</v>
-      </c>
-      <c r="C83" t="s">
-        <v>249</v>
-      </c>
-      <c r="D83" t="s">
-        <v>251</v>
-      </c>
-      <c r="E83" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>120</v>
-      </c>
-      <c r="B84" t="s">
-        <v>33</v>
-      </c>
-      <c r="C84" t="s">
-        <v>250</v>
-      </c>
-      <c r="D84" t="s">
-        <v>4</v>
-      </c>
-      <c r="E84" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>120</v>
-      </c>
-      <c r="B85" t="s">
-        <v>97</v>
-      </c>
-      <c r="C85" t="s">
-        <v>256</v>
-      </c>
-      <c r="D85" t="s">
-        <v>251</v>
-      </c>
-      <c r="E85" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>120</v>
-      </c>
-      <c r="B86" t="s">
-        <v>97</v>
-      </c>
-      <c r="C86" t="s">
-        <v>257</v>
-      </c>
-      <c r="D86" t="s">
-        <v>4</v>
-      </c>
-      <c r="E86" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
-        <v>97</v>
-      </c>
-      <c r="C87" t="s">
-        <v>236</v>
-      </c>
-      <c r="D87" t="s">
-        <v>27</v>
-      </c>
-      <c r="E87" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>120</v>
-      </c>
-      <c r="B88" t="s">
-        <v>34</v>
-      </c>
-      <c r="C88" t="s">
-        <v>263</v>
-      </c>
-      <c r="D88" t="s">
-        <v>251</v>
-      </c>
-      <c r="E88" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>120</v>
-      </c>
-      <c r="B89" t="s">
-        <v>34</v>
-      </c>
-      <c r="C89" t="s">
-        <v>264</v>
-      </c>
-      <c r="D89" t="s">
-        <v>4</v>
-      </c>
-      <c r="E89" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
-        <v>34</v>
-      </c>
-      <c r="C90" t="s">
-        <v>265</v>
-      </c>
-      <c r="D90" t="s">
-        <v>27</v>
-      </c>
-      <c r="E90" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>120</v>
-      </c>
-      <c r="B91" t="s">
-        <v>37</v>
-      </c>
-      <c r="C91" t="s">
-        <v>269</v>
-      </c>
-      <c r="E91" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>120</v>
-      </c>
-      <c r="B92" t="s">
-        <v>37</v>
-      </c>
-      <c r="C92" t="s">
-        <v>365</v>
-      </c>
-      <c r="D92" t="s">
-        <v>109</v>
-      </c>
-      <c r="E92" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>120</v>
-      </c>
-      <c r="B93" t="s">
-        <v>38</v>
-      </c>
-      <c r="C93" t="s">
-        <v>269</v>
-      </c>
-      <c r="E93" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>120</v>
-      </c>
-      <c r="B94" t="s">
-        <v>39</v>
-      </c>
-      <c r="C94" t="s">
-        <v>278</v>
-      </c>
-      <c r="E94" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>120</v>
-      </c>
-      <c r="B95" t="s">
-        <v>45</v>
-      </c>
-      <c r="C95" t="s">
-        <v>279</v>
-      </c>
-      <c r="E95" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>120</v>
-      </c>
-      <c r="B96" t="s">
-        <v>6</v>
-      </c>
-      <c r="C96" t="s">
-        <v>188</v>
-      </c>
-      <c r="E96" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>120</v>
-      </c>
-      <c r="B97" t="s">
-        <v>10</v>
-      </c>
-      <c r="C97" t="s">
-        <v>188</v>
-      </c>
-      <c r="E97" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
-        <v>28</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>14</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
-        <v>14</v>
-      </c>
-      <c r="B102" t="s">
-        <v>8</v>
-      </c>
-      <c r="C102" t="s">
-        <v>286</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B57:B63">
+  <conditionalFormatting sqref="B10:B16">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($B:$B, B57)&gt;1</formula>
+      <formula>COUNTIF($B:$B, B10)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5618,34 +4946,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -5653,54 +4981,54 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished special final E U
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77521C03-936E-42DE-AABE-B2E6431A6169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E1C58A-400C-4BFF-AC9F-A6F92E5B658F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="6" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
@@ -1450,7 +1450,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1473,6 +1473,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3482,8 +3488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C0AE4-7BC5-4B30-B89D-2A08841991C9}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3492,37 +3498,37 @@
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>114</v>
+      <c r="A3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -3530,7 +3536,7 @@
         <v>118</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>122</v>
@@ -3541,87 +3547,87 @@
         <v>118</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>124</v>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>133</v>
+      <c r="A7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>5</v>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>8</v>
+        <v>120</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>130</v>
+      <c r="C12" s="8" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3632,6 +3638,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3662,7 +3669,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3681,7 +3688,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -3722,7 +3729,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -3741,7 +3748,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -3760,7 +3767,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -3782,7 +3789,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -3823,7 +3830,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -3842,7 +3849,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -3861,7 +3868,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -3869,7 +3876,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -3877,7 +3884,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -3885,7 +3892,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>14</v>
       </c>
@@ -3896,7 +3903,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -3904,7 +3911,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -3912,7 +3919,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -3920,7 +3927,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>18</v>
       </c>
@@ -3928,7 +3935,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -3936,7 +3943,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>20</v>
       </c>
@@ -3944,7 +3951,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>21</v>
       </c>
@@ -3952,7 +3959,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>22</v>
       </c>
@@ -3960,7 +3967,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>23</v>
       </c>
@@ -3968,7 +3975,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -3979,7 +3986,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>24</v>
       </c>
@@ -3987,7 +3994,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>24</v>
       </c>
@@ -3998,7 +4005,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>25</v>
       </c>
@@ -4006,7 +4013,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>26</v>
       </c>
@@ -4014,7 +4021,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>27</v>
       </c>
@@ -4022,7 +4029,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>28</v>
       </c>
@@ -4030,7 +4037,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>29</v>
       </c>
@@ -4038,7 +4045,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>30</v>
       </c>
@@ -4046,7 +4053,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>31</v>
       </c>
@@ -4054,7 +4061,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>32</v>
       </c>
@@ -4062,7 +4069,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>33</v>
       </c>
@@ -4070,7 +4077,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>95</v>
       </c>
@@ -4078,7 +4085,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>95</v>
       </c>
@@ -4089,7 +4096,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -4097,7 +4104,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>35</v>
       </c>
@@ -4105,7 +4112,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>36</v>
       </c>
@@ -4113,7 +4120,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>37</v>
       </c>
@@ -4121,7 +4128,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>38</v>
       </c>
@@ -4129,7 +4136,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>39</v>
       </c>
@@ -4137,7 +4144,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>40</v>
       </c>
@@ -4145,7 +4152,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>41</v>
       </c>
@@ -4153,7 +4160,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>42</v>
       </c>
@@ -4161,7 +4168,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>42</v>
       </c>
@@ -4172,7 +4179,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>43</v>
       </c>
@@ -4180,7 +4187,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>44</v>
       </c>
@@ -4188,7 +4195,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>45</v>
       </c>
@@ -4197,7 +4204,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E61" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}"/>
+  <autoFilter ref="A1:E61" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4265,8 +4278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refined the curation strategy and finished N
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E1C58A-400C-4BFF-AC9F-A6F92E5B658F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3A7BF-DF65-4E8E-A43F-66A86079004B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="3" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="6" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicode" sheetId="7" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="367">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1381,6 +1381,26 @@
   </si>
   <si>
     <t>F.med.ngfi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N.init</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U.fin.Cu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N.med.ne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N.med.nu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N with dot under I</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1388,7 +1408,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1416,6 +1436,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1450,7 +1479,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1479,6 +1508,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3488,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C0AE4-7BC5-4B30-B89D-2A08841991C9}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3609,24 +3641,24 @@
       </c>
     </row>
     <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>114</v>
       </c>
     </row>
@@ -3641,7 +3673,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3669,7 +3703,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3677,7 +3711,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -3688,7 +3722,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
@@ -3696,7 +3730,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -3707,7 +3741,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -3718,7 +3752,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -3729,7 +3763,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -3737,7 +3771,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -3748,7 +3782,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -3756,7 +3790,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -3767,7 +3801,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -3775,7 +3809,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3789,7 +3823,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -3797,7 +3831,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>111</v>
       </c>
@@ -3808,7 +3842,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -3819,7 +3853,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -3830,7 +3864,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>9</v>
       </c>
@@ -3838,7 +3872,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -3849,7 +3883,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>11</v>
       </c>
@@ -3857,7 +3891,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -3868,7 +3902,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -3876,7 +3910,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -3884,7 +3918,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -3903,7 +3937,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -3911,7 +3945,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -3919,7 +3953,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -3927,7 +3961,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>18</v>
       </c>
@@ -3935,7 +3969,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -3943,7 +3977,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>20</v>
       </c>
@@ -3951,7 +3985,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>21</v>
       </c>
@@ -3959,7 +3993,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>22</v>
       </c>
@@ -3967,7 +4001,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>23</v>
       </c>
@@ -3986,7 +4020,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>24</v>
       </c>
@@ -4005,7 +4039,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>25</v>
       </c>
@@ -4013,7 +4047,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>26</v>
       </c>
@@ -4021,7 +4055,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>27</v>
       </c>
@@ -4029,7 +4063,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>28</v>
       </c>
@@ -4037,7 +4071,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>29</v>
       </c>
@@ -4045,7 +4079,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>30</v>
       </c>
@@ -4053,7 +4087,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>31</v>
       </c>
@@ -4061,7 +4095,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>32</v>
       </c>
@@ -4069,7 +4103,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>33</v>
       </c>
@@ -4077,7 +4111,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>95</v>
       </c>
@@ -4096,7 +4130,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -4104,7 +4138,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>35</v>
       </c>
@@ -4112,7 +4146,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="51" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>36</v>
       </c>
@@ -4120,7 +4154,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>37</v>
       </c>
@@ -4128,7 +4162,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>38</v>
       </c>
@@ -4136,7 +4170,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>39</v>
       </c>
@@ -4144,7 +4178,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="55" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>40</v>
       </c>
@@ -4152,7 +4186,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>41</v>
       </c>
@@ -4160,7 +4194,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="57" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>42</v>
       </c>
@@ -4179,7 +4213,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>43</v>
       </c>
@@ -4187,7 +4221,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>44</v>
       </c>
@@ -4195,7 +4229,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>45</v>
       </c>
@@ -4206,9 +4240,10 @@
   </sheetData>
   <autoFilter ref="A1:E61" xr:uid="{40E23EE1-FE41-4BE1-BE91-C10F6C805400}">
     <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters blank="1"/>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4276,10 +4311,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4290,7 +4325,7 @@
     <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4298,643 +4333,910 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D11" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C27" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D27" s="8" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D29" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F30" s="8"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E34" s="8" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>353</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C41" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D12" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>183</v>
-      </c>
-      <c r="E21" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>184</v>
-      </c>
-      <c r="E22" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>197</v>
-      </c>
-      <c r="E24" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s">
-        <v>197</v>
-      </c>
-      <c r="D25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>211</v>
-      </c>
-      <c r="D26" t="s">
-        <v>212</v>
-      </c>
-      <c r="E26" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>211</v>
-      </c>
-      <c r="D27" t="s">
-        <v>212</v>
-      </c>
-      <c r="E27" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" t="s">
-        <v>272</v>
-      </c>
-      <c r="D28" t="s">
-        <v>227</v>
-      </c>
-      <c r="E28" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" t="s">
-        <v>273</v>
-      </c>
-      <c r="D29" t="s">
-        <v>228</v>
-      </c>
-      <c r="E29" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>270</v>
-      </c>
-      <c r="D30" t="s">
-        <v>227</v>
-      </c>
-      <c r="E30" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" t="s">
-        <v>271</v>
-      </c>
-      <c r="D31" t="s">
-        <v>228</v>
-      </c>
-      <c r="E31" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>118</v>
-      </c>
-      <c r="B33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" t="s">
-        <v>236</v>
-      </c>
-      <c r="E33" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" t="s">
-        <v>275</v>
-      </c>
-      <c r="E34" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s">
-        <v>274</v>
-      </c>
-      <c r="E35" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>247</v>
-      </c>
-      <c r="D36" t="s">
-        <v>249</v>
-      </c>
-      <c r="E36" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" t="s">
-        <v>248</v>
-      </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" t="s">
-        <v>254</v>
-      </c>
-      <c r="D38" t="s">
-        <v>249</v>
-      </c>
-      <c r="E38" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" t="s">
-        <v>255</v>
-      </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-      <c r="E39" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>95</v>
-      </c>
-      <c r="C40" t="s">
-        <v>234</v>
-      </c>
-      <c r="D40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" t="s">
-        <v>261</v>
-      </c>
-      <c r="D41" t="s">
-        <v>249</v>
-      </c>
-      <c r="E41" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" t="s">
-        <v>262</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" t="s">
-        <v>263</v>
-      </c>
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" t="s">
-        <v>267</v>
-      </c>
-      <c r="E44" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>118</v>
-      </c>
-      <c r="B45" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" t="s">
-        <v>361</v>
-      </c>
-      <c r="D45" t="s">
-        <v>107</v>
-      </c>
-      <c r="E45" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" t="s">
-        <v>267</v>
-      </c>
-      <c r="E46" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" t="s">
-        <v>276</v>
-      </c>
-      <c r="E47" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" t="s">
-        <v>45</v>
-      </c>
-      <c r="C48" t="s">
-        <v>277</v>
-      </c>
-      <c r="E48" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" t="s">
-        <v>186</v>
-      </c>
-      <c r="E49" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>118</v>
-      </c>
-      <c r="B50" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" t="s">
-        <v>186</v>
-      </c>
-      <c r="E50" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>28</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="C62" s="8" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" t="s">
-        <v>284</v>
-      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B10:B16">
+  <conditionalFormatting sqref="B28:B29 B19:B23">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($B:$B, B10)&gt;1</formula>
+      <formula>COUNTIF($B:$B, B19)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refined letters under the round letters
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C3A7BF-DF65-4E8E-A43F-66A86079004B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD13C05-4DB5-4431-B226-43A8AC83A6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="6" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Canvas" sheetId="10" r:id="rId4"/>
     <sheet name="Final" sheetId="3" r:id="rId5"/>
     <sheet name="Isolated" sheetId="4" r:id="rId6"/>
-    <sheet name="RLig" sheetId="5" r:id="rId7"/>
+    <sheet name="Refine" sheetId="5" r:id="rId7"/>
     <sheet name="Kerning" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="377">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1134,9 +1134,6 @@
   </si>
   <si>
     <t>U.fin.Xnu</t>
-  </si>
-  <si>
-    <t>U.fin.Xnu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1400,7 +1397,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>N with dot under I</t>
+    <t>Contextual Substitution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Required Ligature</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Preffix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Suffix</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E.fin, E.med</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U.med U.fin.Cu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E.med, E.fin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U.med, U.fin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I.med I.med.ai V.init V.med V.med.bv Y.coda F.med.fa W.med</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N.init.ne N.med.ne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N.init.nu N.med.nu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1443,8 +1484,9 @@
     </font>
     <font>
       <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1479,7 +1521,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1510,21 +1552,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1890,15 +1940,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B2" s="4">
         <v>1820</v>
@@ -1906,15 +1956,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B4" s="4">
         <v>1873</v>
@@ -1922,15 +1972,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B6" s="4">
         <v>1823</v>
@@ -1938,7 +1988,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B7" s="4">
         <v>1860</v>
@@ -1946,7 +1996,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B8" s="4">
         <v>1861</v>
@@ -1954,15 +2004,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>298</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B10" s="4">
         <v>1828</v>
@@ -1970,7 +2020,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B11" s="4">
         <v>1829</v>
@@ -1978,23 +2028,23 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B14" s="4">
         <v>1866</v>
@@ -2002,7 +2052,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B15" s="4">
         <v>1874</v>
@@ -2010,15 +2060,15 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>308</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B17" s="4">
         <v>1864</v>
@@ -2026,7 +2076,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B18" s="4">
         <v>1865</v>
@@ -2034,7 +2084,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B19" s="4">
         <v>1830</v>
@@ -2042,7 +2092,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B20" s="4">
         <v>1867</v>
@@ -2050,7 +2100,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B21" s="4">
         <v>1868</v>
@@ -2058,7 +2108,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B22" s="4">
         <v>1869</v>
@@ -2066,23 +2116,23 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>316</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>318</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B25" s="4">
         <v>1834</v>
@@ -2090,7 +2140,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B26" s="4">
         <v>1835</v>
@@ -2098,15 +2148,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>322</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B28" s="4">
         <v>1836</v>
@@ -2114,31 +2164,31 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>325</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>327</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>329</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B32" s="4">
         <v>1875</v>
@@ -2146,7 +2196,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B33" s="4">
         <v>1837</v>
@@ -2154,7 +2204,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B34" s="4">
         <v>1876</v>
@@ -2162,15 +2212,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>334</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B36" s="4">
         <v>1838</v>
@@ -2178,66 +2228,66 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>337</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>339</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>341</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>343</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>347</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -2467,7 +2517,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2486,7 +2536,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2767,7 +2817,7 @@
         <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2812,7 +2862,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2910,7 +2960,7 @@
         <v>191</v>
       </c>
       <c r="E11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3002,7 +3052,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4311,10 +4361,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4325,672 +4375,551 @@
     <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>232</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="6" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="C12" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>375</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>183</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>375</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>358</v>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>358</v>
-      </c>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>358</v>
+        <v>376</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>196</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>358</v>
+        <v>364</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>283</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>362</v>
+      </c>
+      <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>358</v>
+        <v>282</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>284</v>
-      </c>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>282</v>
-      </c>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="E28" s="8"/>
+        <v>197</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>357</v>
+      </c>
       <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>358</v>
-      </c>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8" t="s">
-        <v>358</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>5</v>
+        <v>352</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8" t="s">
-        <v>358</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8" t="s">
-        <v>358</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8" t="s">
-        <v>358</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
+      <c r="A34" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="B34" s="8" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>197</v>
+        <v>27</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>358</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
-      <c r="B35" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>358</v>
-      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F45" s="8"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>249</v>
-      </c>
       <c r="E47" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F47" s="8"/>
     </row>
@@ -4999,32 +4928,34 @@
         <v>118</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>4</v>
+        <v>227</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="8"/>
+      <c r="A49" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="B49" s="8" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>234</v>
+        <v>273</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F49" s="8"/>
     </row>
@@ -5033,16 +4964,16 @@
         <v>118</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>249</v>
+        <v>227</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F50" s="8"/>
     </row>
@@ -5051,32 +4982,32 @@
         <v>118</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>4</v>
+        <v>228</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
+      <c r="A52" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="B52" s="8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="D52" s="8"/>
       <c r="E52" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F52" s="8"/>
     </row>
@@ -5085,14 +5016,14 @@
         <v>118</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>267</v>
+        <v>236</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F53" s="8"/>
     </row>
@@ -5101,16 +5032,14 @@
         <v>118</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>361</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>107</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="D54" s="8"/>
       <c r="E54" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F54" s="8"/>
     </row>
@@ -5119,14 +5048,14 @@
         <v>118</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F55" s="8"/>
     </row>
@@ -5135,14 +5064,16 @@
         <v>118</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="D56" s="8"/>
+        <v>247</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>249</v>
+      </c>
       <c r="E56" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F56" s="8"/>
     </row>
@@ -5151,14 +5082,16 @@
         <v>118</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="D57" s="8"/>
+        <v>248</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E57" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F57" s="8"/>
     </row>
@@ -5167,14 +5100,16 @@
         <v>118</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>6</v>
+        <v>95</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="D58" s="8"/>
+        <v>254</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>249</v>
+      </c>
       <c r="E58" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F58" s="8"/>
     </row>
@@ -5183,60 +5118,251 @@
         <v>118</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="D59" s="8"/>
+        <v>255</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E59" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F59" s="8"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="B60" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>357</v>
+      </c>
       <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="A61" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>357</v>
+      </c>
       <c r="F61" s="8"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>5</v>
+        <v>118</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>357</v>
+      </c>
       <c r="F62" s="8"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="B63" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>357</v>
+      </c>
       <c r="F63" s="8"/>
     </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F66" s="8"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F69" s="8"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="8"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="8"/>
+    </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A20:D20"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B28:B29 B19:B23">
+  <conditionalFormatting sqref="B39:B40 B30:B34">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($B:$B, B19)&gt;1</formula>
+      <formula>COUNTIF($B:$B, B30)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5261,10 +5387,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Debug N's dot doesn't avert medial I
</commit_message>
<xml_diff>
--- a/Contribution/Transformation.xlsx
+++ b/Contribution/Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Manju Gisun\Modern Ginguler Font\GitHub\ManchuTextFont\Contribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF264F25-9165-4602-9549-6EF6EA9D0AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED1C866-8A61-4FDD-AD18-564C4F34BDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" activeTab="6" xr2:uid="{B35BB998-90F8-4227-BD9E-85BAC482EB58}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="383">
   <si>
     <t>Substitue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1454,6 +1454,18 @@
   </si>
   <si>
     <t>Deconflict down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L.med F.med.fa F.fin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IY.init</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D.init.da</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4375,8 +4387,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4522636C-59D4-401B-8C2E-91A4263478BC}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4953,7 +4966,7 @@
         <v>235</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>8</v>
+        <v>192</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>197</v>
@@ -4972,114 +4985,106 @@
       <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="B49" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="8"/>
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="B50" s="8" t="s">
-        <v>351</v>
+        <v>192</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50" s="8"/>
+        <v>380</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>197</v>
+      </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="B51" s="8" t="s">
-        <v>134</v>
+        <v>381</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51" s="8"/>
+        <v>380</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>351</v>
+      </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
-        <v>95</v>
-      </c>
       <c r="B52" s="8" t="s">
-        <v>100</v>
+        <v>382</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="8"/>
+        <v>380</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="B53" s="8" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D53" s="8"/>
+        <v>380</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="B54" s="8" t="s">
-        <v>197</v>
+        <v>102</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54" s="8"/>
+        <v>380</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>105</v>
+      </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>95</v>
-      </c>
       <c r="B55" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D55" s="8"/>
       <c r="E55" s="8"/>
       <c r="F55" s="8"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="B56" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D56" s="8"/>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
     </row>
@@ -5177,9 +5182,9 @@
     <mergeCell ref="A11:D11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B49:B53">
+  <conditionalFormatting sqref="D51:D54 D49">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>COUNTIF($B:$B, B49)&gt;1</formula>
+      <formula>COUNTIF($B:$B, D49)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>